<commit_message>
Created player outfit manager
</commit_message>
<xml_diff>
--- a/4 Koalas Dress Up Game/Assets/Editor/ClothingData.xlsx
+++ b/4 Koalas Dress Up Game/Assets/Editor/ClothingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etern\OneDrive\Documents\GitHub\4-Koalas_Dress-Up-Game\4 Koalas Dress Up Game\Assets\Editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3A220B-A74D-430B-8FFE-952E8397DA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEF25F1-3419-4842-89AE-9A70489093CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CEBD6C52-8314-4506-A5BF-7640DC283251}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CEBD6C52-8314-4506-A5BF-7640DC283251}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Clothing Types</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>TestShoes</t>
+  </si>
+  <si>
+    <t>TopHat</t>
+  </si>
+  <si>
+    <t>TankTop</t>
+  </si>
+  <si>
+    <t>Jorts</t>
+  </si>
+  <si>
+    <t>Sneakers</t>
   </si>
 </sst>
 </file>
@@ -181,8 +193,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4EC23CB2-099D-4E1D-80BF-78AF0C08E066}" name="ClothingItems" displayName="ClothingItems" ref="C4:D8" totalsRowShown="0">
-  <autoFilter ref="C4:D8" xr:uid="{4EC23CB2-099D-4E1D-80BF-78AF0C08E066}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4EC23CB2-099D-4E1D-80BF-78AF0C08E066}" name="ClothingItems" displayName="ClothingItems" ref="C4:D12" totalsRowShown="0">
+  <autoFilter ref="C4:D12" xr:uid="{4EC23CB2-099D-4E1D-80BF-78AF0C08E066}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{80AFD55D-4E92-4DB9-AF0A-2FEC20EFA2AA}" name="Name"/>
     <tableColumn id="2" xr3:uid="{83ADDADE-7857-4065-A606-205D0692CC3F}" name="Type"/>
@@ -508,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF4EFA30-489C-4F29-AECE-FE7BBEAAF235}">
-  <dimension ref="C4:D8"/>
+  <dimension ref="C4:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,6 +565,38 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -568,7 +612,7 @@
           <x14:formula1>
             <xm:f>Enumerations!$B$4:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D8</xm:sqref>
+          <xm:sqref>D5:D12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Added sprites and sounds (milestone 1 build)
</commit_message>
<xml_diff>
--- a/4 Koalas Dress Up Game/Assets/Editor/ClothingData.xlsx
+++ b/4 Koalas Dress Up Game/Assets/Editor/ClothingData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etern\OneDrive\Documents\GitHub\4-Koalas_Dress-Up-Game\4 Koalas Dress Up Game\Assets\Editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEF25F1-3419-4842-89AE-9A70489093CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EAB23D-F4F3-4825-97B3-CE90A212513A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CEBD6C52-8314-4506-A5BF-7640DC283251}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CEBD6C52-8314-4506-A5BF-7640DC283251}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,16 +72,16 @@
     <t>TestShoes</t>
   </si>
   <si>
-    <t>TopHat</t>
-  </si>
-  <si>
-    <t>TankTop</t>
-  </si>
-  <si>
-    <t>Jorts</t>
-  </si>
-  <si>
-    <t>Sneakers</t>
+    <t>Afro</t>
+  </si>
+  <si>
+    <t>DiscoPants</t>
+  </si>
+  <si>
+    <t>DiscoShirt</t>
+  </si>
+  <si>
+    <t>DiscoShoes</t>
   </si>
 </sst>
 </file>
@@ -523,12 +523,15 @@
   <dimension ref="C4:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -536,7 +539,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>7</v>
       </c>
@@ -544,7 +547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>8</v>
       </c>
@@ -552,7 +555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>9</v>
       </c>
@@ -560,7 +563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>10</v>
       </c>
@@ -568,7 +571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>11</v>
       </c>
@@ -576,23 +579,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>14</v>
       </c>
@@ -628,33 +631,33 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>

</xml_diff>